<commit_message>
add - management commands - employee job, level, and specialty
</commit_message>
<xml_diff>
--- a/core/seed_employees_employeestatus.xlsx
+++ b/core/seed_employees_employeestatus.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan.cheng\Documents\Visual Studio Code\Django\p_sys01_repo01\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE46D90-FF39-41BD-A489-4C640101CE62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F572D6A-8927-4B6B-BE10-804D095A1122}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="new_departments_department" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -880,9 +880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>